<commit_message>
update: override data for VIT5
</commit_message>
<xml_diff>
--- a/data/input/Final_Dataset.xlsx
+++ b/data/input/Final_Dataset.xlsx
@@ -1848,7 +1848,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1863,7 +1863,6 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2376,7 +2375,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E13" zoomScale="100" workbookViewId="0">
       <selection activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
@@ -3041,66 +3040,70 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="I21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="2">
         <v>65</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F22" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I22" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" t="s">
+      <c r="I22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="2">
         <v>65</v>
       </c>
     </row>
@@ -3329,66 +3332,70 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F30" t="s">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I30" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="I30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="3">
         <v>65</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="3">
         <v>2</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F31" t="s">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I31" t="s">
-        <v>17</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="I31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="3">
         <v>65</v>
       </c>
     </row>
@@ -12940,7 +12947,7 @@
       </c>
     </row>
     <row r="317">
-      <c r="A317" s="8" t="s">
+      <c r="A317" s="2" t="s">
         <v>326</v>
       </c>
       <c r="B317" s="2">

</xml_diff>